<commit_message>
Part information updates and corrections
- Earth wire is now 16awg.
- Lots of added links and corrections in the part list.
- Removed a few stale entries.
- Freshened /Scripts readme.
</commit_message>
<xml_diff>
--- a/Docs/ID Lists.xlsx
+++ b/Docs/ID Lists.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jon\Documents\3D Print\Clockmaker\clock-3\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74A8E967-AC3D-4C34-8657-914527A169D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0223C48F-B91E-4A39-976F-6B0F5118D1B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{2BA3904D-48D5-4484-9C88-BD860323DFB0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{2BA3904D-48D5-4484-9C88-BD860323DFB0}"/>
   </bookViews>
   <sheets>
     <sheet name="Electrical IDs" sheetId="1" r:id="rId1"/>
@@ -1583,9 +1583,6 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right/>
@@ -1628,6 +1625,9 @@
         <vertical/>
         <horizontal/>
       </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1672,7 +1672,7 @@
     <tableColumn id="3" xr3:uid="{12F9C25F-8EE1-4903-9829-BB393B754AE2}" name="AWG"/>
     <tableColumn id="4" xr3:uid="{9DAEE46D-2720-4E12-B7C7-7347C849AB98}" name="Pin Count"/>
     <tableColumn id="5" xr3:uid="{09BB7B9C-817F-47EC-B02A-087CF00AE010}" name="Len (cm)"/>
-    <tableColumn id="10" xr3:uid="{32FDE131-45FB-4569-9AD2-489ACB6C5A82}" name="Column1" dataDxfId="0">
+    <tableColumn id="10" xr3:uid="{32FDE131-45FB-4569-9AD2-489ACB6C5A82}" name="Column1" dataDxfId="5">
       <calculatedColumnFormula>Table3[[#This Row],[Pin Count]]*Table3[[#This Row],[Len (cm)]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="6" xr3:uid="{41A61DCB-EB69-4ABD-AC8C-6A79DAAE3294}" name="Conn A"/>
@@ -1714,12 +1714,12 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{A69B5B3E-6862-404E-BD2D-269E8426AC20}" name="Table5" displayName="Table5" ref="A1:F97" totalsRowCount="1">
   <autoFilter ref="A1:F96" xr:uid="{A69B5B3E-6862-404E-BD2D-269E8426AC20}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{74644EAE-7BA4-4FB3-8AD5-3C78AE3D81AD}" name="PN" totalsRowLabel="Total" dataDxfId="5" totalsRowDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{93DF1DAA-9D24-4594-B29D-2B6C121D089A}" name="Description" dataDxfId="3" totalsRowDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{74644EAE-7BA4-4FB3-8AD5-3C78AE3D81AD}" name="PN" totalsRowLabel="Total" dataDxfId="4" totalsRowDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{93DF1DAA-9D24-4594-B29D-2B6C121D089A}" name="Description" dataDxfId="2" totalsRowDxfId="1"/>
     <tableColumn id="3" xr3:uid="{ADFE1D10-4761-4B07-8EB7-A4DDEEF5308B}" name="Material"/>
     <tableColumn id="4" xr3:uid="{A91C48D7-D2C5-4A18-9E62-A24A122EE139}" name="HS Inserts"/>
     <tableColumn id="5" xr3:uid="{0112B1B1-C190-46E0-8D0F-19B785DD6A37}" name="Qty"/>
-    <tableColumn id="6" xr3:uid="{6618CC07-9735-42B6-AD61-ED6CD4EA2E17}" name="Subtotal" totalsRowFunction="sum" dataDxfId="1">
+    <tableColumn id="6" xr3:uid="{6618CC07-9735-42B6-AD61-ED6CD4EA2E17}" name="Subtotal" totalsRowFunction="sum" dataDxfId="0">
       <calculatedColumnFormula>Table5[[#This Row],[HS Inserts]]*Table5[[#This Row],[Qty]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2477,7 +2477,7 @@
   <dimension ref="A1:I59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2759,34 +2759,37 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>103</v>
+        <v>165</v>
       </c>
       <c r="B10" t="s">
-        <v>22</v>
+        <v>163</v>
       </c>
       <c r="C10">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E10">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="F10">
         <f>Table3[[#This Row],[Pin Count]]*Table3[[#This Row],[Len (cm)]]</f>
-        <v>110</v>
+        <v>60</v>
       </c>
       <c r="G10" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="H10" t="s">
-        <v>483</v>
+        <v>149</v>
+      </c>
+      <c r="I10" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B11" t="s">
         <v>22</v>
@@ -2798,14 +2801,14 @@
         <v>2</v>
       </c>
       <c r="E11">
-        <v>150</v>
+        <v>55</v>
       </c>
       <c r="F11">
         <f>Table3[[#This Row],[Pin Count]]*Table3[[#This Row],[Len (cm)]]</f>
-        <v>300</v>
+        <v>110</v>
       </c>
       <c r="G11" t="s">
-        <v>484</v>
+        <v>143</v>
       </c>
       <c r="H11" t="s">
         <v>483</v>
@@ -2813,10 +2816,10 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>159</v>
+        <v>104</v>
       </c>
       <c r="B12" t="s">
-        <v>154</v>
+        <v>22</v>
       </c>
       <c r="C12">
         <v>20</v>
@@ -2825,50 +2828,47 @@
         <v>2</v>
       </c>
       <c r="E12">
-        <v>55</v>
+        <v>150</v>
       </c>
       <c r="F12">
         <f>Table3[[#This Row],[Pin Count]]*Table3[[#This Row],[Len (cm)]]</f>
-        <v>110</v>
+        <v>300</v>
       </c>
       <c r="G12" t="s">
-        <v>149</v>
+        <v>484</v>
       </c>
       <c r="H12" t="s">
-        <v>143</v>
-      </c>
-      <c r="I12" t="s">
-        <v>161</v>
+        <v>483</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="B13" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="C13">
         <v>20</v>
       </c>
       <c r="D13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E13">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="F13">
         <f>Table3[[#This Row],[Pin Count]]*Table3[[#This Row],[Len (cm)]]</f>
-        <v>60</v>
+        <v>110</v>
       </c>
       <c r="G13" t="s">
         <v>149</v>
       </c>
       <c r="H13" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="I13" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>